<commit_message>
WorksheetTemplate.xlsx now has alphabetical Strengths listing
</commit_message>
<xml_diff>
--- a/src/main/resources/WorksheetTemplate.xlsx
+++ b/src/main/resources/WorksheetTemplate.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\secondphase\parillume\src\main\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tomma\saige\tmp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B0F4C60-A8C2-4251-B961-9B507C896A3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A584174-7E0C-4A35-AA61-969683C78EB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{EF544F7F-FE12-4575-9343-7880C024C4F5}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{EF544F7F-FE12-4575-9343-7880C024C4F5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="55">
   <si>
     <t>Name</t>
   </si>
@@ -174,9 +174,6 @@
   </si>
   <si>
     <t>Margolis</t>
-  </si>
-  <si>
-    <t>This Strengths order matches the order on the team CliftonStrengths chart</t>
   </si>
   <si>
     <t>SELF_ASSURANCE</t>
@@ -587,8 +584,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3580F207-1E93-4B18-BC79-037CEC09EC36}">
   <dimension ref="A1:J53"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -618,25 +615,25 @@
         <v>18</v>
       </c>
       <c r="E1" t="s">
+        <v>51</v>
+      </c>
+      <c r="F1" t="s">
         <v>52</v>
-      </c>
-      <c r="F1" t="s">
-        <v>53</v>
       </c>
       <c r="G1" t="s">
         <v>19</v>
       </c>
       <c r="H1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="I1" t="s">
+        <v>46</v>
+      </c>
+      <c r="J1" t="s">
         <v>47</v>
       </c>
-      <c r="J1" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" ht="216" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:10" ht="187.2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>43</v>
       </c>
@@ -650,20 +647,20 @@
         <v>5</v>
       </c>
       <c r="E2" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>54</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>55</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>42</v>
       </c>
       <c r="H2" s="1"/>
       <c r="I2" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="J2" s="1" t="s">
         <v>49</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
@@ -671,7 +668,7 @@
         <v>44</v>
       </c>
       <c r="B3">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C3" t="s">
         <v>15</v>
@@ -679,7 +676,7 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B4">
-        <v>19</v>
+        <v>9</v>
       </c>
       <c r="C4" t="s">
         <v>16</v>
@@ -687,7 +684,7 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B5">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="C5" t="s">
         <v>17</v>
@@ -698,187 +695,185 @@
         <v>41</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B7" t="s">
-        <v>45</v>
-      </c>
-    </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
-        <v>2</v>
+        <v>21</v>
       </c>
       <c r="E8" s="3"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
-        <v>20</v>
+        <v>4</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
-        <v>3</v>
+        <v>22</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
-        <v>10</v>
+        <v>2</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
-        <v>32</v>
+        <v>8</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
-        <v>34</v>
+        <v>24</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B15" t="s">
-        <v>40</v>
+        <v>5</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
-        <v>4</v>
+        <v>26</v>
       </c>
     </row>
     <row r="17" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B17" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="18" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B18" t="s">
-        <v>5</v>
+        <v>27</v>
       </c>
       <c r="E18" s="3"/>
     </row>
     <row r="19" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B19" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
     </row>
     <row r="20" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B20" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
     </row>
     <row r="21" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B21" t="s">
-        <v>46</v>
+        <v>6</v>
       </c>
     </row>
     <row r="22" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B22" t="s">
-        <v>39</v>
+        <v>7</v>
       </c>
     </row>
     <row r="23" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B23" t="s">
-        <v>41</v>
+        <v>29</v>
       </c>
     </row>
     <row r="24" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B24" t="s">
-        <v>21</v>
+        <v>30</v>
       </c>
     </row>
     <row r="25" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B25" t="s">
-        <v>23</v>
+        <v>3</v>
       </c>
     </row>
     <row r="26" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B26" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="27" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B27" t="s">
-        <v>27</v>
+        <v>10</v>
       </c>
     </row>
     <row r="28" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B28" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
     </row>
     <row r="29" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B29" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="30" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B30" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="31" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B31" t="s">
-        <v>12</v>
+        <v>32</v>
       </c>
     </row>
     <row r="32" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B32" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
     </row>
     <row r="33" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B33" t="s">
-        <v>22</v>
+        <v>35</v>
       </c>
     </row>
     <row r="34" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B34" t="s">
-        <v>25</v>
+        <v>36</v>
       </c>
     </row>
     <row r="35" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B35" t="s">
-        <v>6</v>
+        <v>37</v>
       </c>
     </row>
     <row r="36" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B36" t="s">
-        <v>29</v>
+        <v>12</v>
       </c>
     </row>
     <row r="37" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B37" t="s">
-        <v>9</v>
+        <v>38</v>
       </c>
     </row>
     <row r="38" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B38" t="s">
-        <v>33</v>
+        <v>45</v>
       </c>
     </row>
     <row r="39" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B39" t="s">
-        <v>11</v>
+        <v>39</v>
       </c>
     </row>
     <row r="40" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B40" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
     </row>
     <row r="41" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B41" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
     </row>
     <row r="53" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E53" s="3"/>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B8:B41">
+    <sortCondition ref="B8:B41"/>
+  </sortState>
   <hyperlinks>
     <hyperlink ref="I2" r:id="rId1" xr:uid="{E8639232-FA4D-4368-97B0-AFF8FDE0296D}"/>
   </hyperlinks>

</xml_diff>